<commit_message>
More details added to BOM
</commit_message>
<xml_diff>
--- a/Hardware/production/home_bom.xlsx
+++ b/Hardware/production/home_bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="275">
   <si>
     <t>Qty</t>
   </si>
@@ -828,6 +828,27 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Pins</t>
+  </si>
+  <si>
+    <t>SMT?</t>
+  </si>
+  <si>
+    <t>SMT Pads</t>
+  </si>
+  <si>
+    <t>TH Pads</t>
+  </si>
+  <si>
+    <t>IC Pads</t>
+  </si>
+  <si>
+    <t>IC?</t>
+  </si>
+  <si>
+    <t>IC SMT Pads</t>
   </si>
 </sst>
 </file>
@@ -872,7 +893,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -909,11 +930,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -922,9 +952,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -946,6 +973,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1226,10 +1260,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K65"/>
+  <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,43 +1271,58 @@
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="62.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.85546875" customWidth="1"/>
-    <col min="11" max="11" width="57.7109375" customWidth="1"/>
+    <col min="4" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" customWidth="1"/>
+    <col min="7" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="62.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="21.140625" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.85546875" customWidth="1"/>
+    <col min="17" max="17" width="57.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>215</v>
       </c>
@@ -1281,1848 +1330,3066 @@
         <v>41472</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="12" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="J6" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="12" t="s">
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="N6" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="O6" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="P6" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="Q6" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
-        <v>1</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="C7" s="13" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>1</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="12">
+        <v>2</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="G7" s="12">
+        <f>IF(B7="Y",IF(E7="Y",IF(F7="N",D7*A7,0),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="12">
+        <f>IF(B7="Y",IF(E7="Y",IF(F7="Y",D7*A7,0),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="12">
+        <f>IF(B7="Y",IF(E7="N",D7*A7,0),0)</f>
+        <v>2</v>
+      </c>
+      <c r="J7" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="K7" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" s="14">
+      <c r="L7" s="12"/>
+      <c r="M7" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="13">
         <v>1012166</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="O7" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="P7" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="K7" s="13"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>1</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="Q7" s="12"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7">
+        <v>2</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" ref="G8:G61" si="0">IF(B8="Y",IF(E8="Y",IF(F8="N",D8*A8,0),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="shared" ref="H8:H61" si="1">IF(B8="Y",IF(E8="Y",IF(F8="Y",D8*A8,0),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="shared" ref="I8:I61" si="2">IF(B8="Y",IF(E8="N",D8*A8,0),0)</f>
+        <v>2</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="K8" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="L8" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" s="9">
+      <c r="M8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="8">
         <v>1298246</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="O8" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="P8" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>1</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="Q8" s="7"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J9" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="K9" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="7">
+      <c r="L9" s="5"/>
+      <c r="M9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="6">
         <v>1192513</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="O9" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="P9" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>2</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="Q9" s="5"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>2</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="7">
+        <v>2</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="K10" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="L10" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" s="9">
+      <c r="M10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="8">
         <v>1856141</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="O10" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="P10" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="K10" s="8"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="Q10" s="7"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="5">
+        <v>2</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="H11" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="K11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="L11" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="M11" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="N11" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="O11" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="P11" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>1</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C12" s="8" t="s">
+      <c r="Q11" s="5"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>1</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H12" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="K12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="L12" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" s="9">
+      <c r="M12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N12" s="8">
         <v>1244342</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="O12" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="P12" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="K12" s="8"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="Q12" s="7"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <v>5</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="K13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="L13" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="M13" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="N13" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="O13" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="P13" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>2</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C14" s="8" t="s">
+      <c r="Q13" s="5"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>2</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="7">
+        <v>2</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G14" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H14" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="K14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="L14" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="G14" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" s="9">
+      <c r="M14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N14" s="8">
         <v>1539489</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="O14" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="P14" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="K14" s="8"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>1</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="Q14" s="7"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5">
+        <v>2</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G15" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H15" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="K15" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="L15" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H15" s="7">
+      <c r="M15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N15" s="6">
         <v>9695877</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="O15" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="P15" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="Q15" s="5"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
         <v>3</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C16" s="8" t="s">
+      <c r="B16" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="7">
+        <v>2</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H16" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="K16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="L16" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="M16" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="N16" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="O16" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="P16" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="K16" s="8"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>1</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="Q16" s="7"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>1</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="5">
+        <v>3</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H17" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="K17" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" s="7">
+      <c r="L17" s="5"/>
+      <c r="M17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17" s="6">
         <v>1689863</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="O17" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="P17" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>2</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="Q17" s="5"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>2</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="7">
+        <v>2</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G18" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H18" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="K18" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="L18" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="G18" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="9">
+      <c r="M18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N18" s="8">
         <v>1336556</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="O18" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="P18" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>1</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="Q18" s="7"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>1</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H19" s="7">
-        <v>9550216</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>182</v>
+      <c r="D19" s="5">
+        <v>2</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H19" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <v>1</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="K19" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N19" s="6">
+        <v>9550216</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="P19" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>1</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H20" s="9">
-        <v>1625280</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>203</v>
+      <c r="D20" s="7">
+        <v>2</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G20" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H20" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J20" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="K20" s="8"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>1</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="K20" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N20" s="8">
+        <v>1625280</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="P20" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q20" s="7"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>1</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H21" s="7">
-        <v>8735654</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>170</v>
+      <c r="D21" s="5">
+        <v>2</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H21" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
-        <v>1</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C22" s="8" t="s">
+      <c r="K21" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N21" s="6">
+        <v>8735654</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q21" s="5"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>1</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H22" s="9">
-        <v>1843695</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>188</v>
+      <c r="D22" s="7">
+        <v>2</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G22" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H22" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J22" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="K22" s="8"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
+      <c r="K22" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N22" s="8">
+        <v>1843695</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="P22" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q22" s="7"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
         <v>3</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="B23" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="5">
+        <v>3</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G23" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="5">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="J23" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="K23" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6" t="s">
+      <c r="L23" s="5"/>
+      <c r="M23" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="N23" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="O23" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J23" s="7" t="s">
+      <c r="P23" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
-        <v>1</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C24" s="8" t="s">
+      <c r="Q23" s="5"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>1</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="7">
+        <v>16</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G24" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="7">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="J24" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="K24" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="L24" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="M24" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="N24" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="O24" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="J24" s="8" t="s">
+      <c r="P24" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="K24" s="8" t="s">
+      <c r="Q24" s="7" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
-        <v>1</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C25" s="6" t="s">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>1</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H25" s="7">
-        <v>2115059</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>195</v>
+      <c r="D25" s="5">
+        <v>48</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G25" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="5">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="I25" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
-        <v>1</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C26" s="8" t="s">
+      <c r="K25" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N25" s="6">
+        <v>2115059</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="P25" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q25" s="5"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>1</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="7">
+        <v>8</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G26" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="7">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I26" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="K26" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="L26" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G26" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H26" s="9">
+      <c r="M26" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N26" s="8">
         <v>1825302</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="O26" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="J26" s="8" t="s">
+      <c r="P26" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="K26" s="8"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
-        <v>1</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C27" s="6" t="s">
+      <c r="Q26" s="7"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>1</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="5">
+        <v>8</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G27" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="5">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I27" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="K27" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="L27" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="G27" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H27" s="7">
+      <c r="M27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N27" s="6">
         <v>8638756</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="O27" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="J27" s="6" t="s">
+      <c r="P27" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="K27" s="6"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
-        <v>1</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C28" s="8" t="s">
+      <c r="Q27" s="5"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="8" t="s">
+      <c r="D28" s="7">
+        <v>6</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G28" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="7">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J28" s="8"/>
+      <c r="K28" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="L28" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="M28" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="N28" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="O28" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="J28" s="8" t="s">
+      <c r="P28" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="K28" s="8"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
-        <v>1</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C29" s="6" t="s">
+      <c r="Q28" s="7"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>1</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="6" t="s">
+      <c r="D29" s="5">
+        <v>7</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G29" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="5">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J29" s="6"/>
+      <c r="K29" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="L29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H29" s="7">
+      <c r="M29" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N29" s="6">
         <v>588763</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="O29" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="J29" s="6" t="s">
+      <c r="P29" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="K29" s="6"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
-        <v>1</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C30" s="8" t="s">
+      <c r="Q29" s="5"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>1</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="7">
+        <v>2</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G30" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H30" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="K30" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H30" s="9">
+      <c r="L30" s="7"/>
+      <c r="M30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N30" s="8">
         <v>1612709</v>
       </c>
-      <c r="I30" s="8" t="s">
+      <c r="O30" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="J30" s="8" t="s">
+      <c r="P30" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="K30" s="8"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
-        <v>1</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="Q30" s="7"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>1</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="5">
+        <v>2</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G31" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H31" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="K31" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="L31" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G31" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H31" s="7">
+      <c r="M31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N31" s="6">
         <v>1929706</v>
       </c>
-      <c r="I31" s="6" t="s">
+      <c r="O31" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="J31" s="6" t="s">
+      <c r="P31" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="K31" s="6"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
-        <v>1</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="C32" s="8" t="s">
+      <c r="Q31" s="5"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>1</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="7">
+        <v>2</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G32" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="K32" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="L32" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="G32" s="8"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8" t="s">
+      <c r="M32" s="7"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
-        <v>1</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C33" s="6" t="s">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>1</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="6" t="s">
+      <c r="D33" s="5">
+        <v>4</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G33" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="5">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="J33" s="6"/>
+      <c r="K33" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="L33" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H33" s="7" t="s">
+      <c r="M33" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N33" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I33" s="6" t="s">
+      <c r="O33" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J33" s="6" t="s">
+      <c r="P33" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="K33" s="6"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
-        <v>1</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C34" s="8" t="s">
+      <c r="Q33" s="5"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>1</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="7">
+        <v>2</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G34" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I34" s="7">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J34" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="K34" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H34" s="9">
+      <c r="L34" s="7"/>
+      <c r="M34" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N34" s="8">
         <v>9350551</v>
       </c>
-      <c r="I34" s="8" t="s">
+      <c r="O34" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="J34" s="8" t="s">
+      <c r="P34" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="K34" s="8"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="6">
-        <v>1</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C35" s="6" t="s">
+      <c r="Q34" s="7"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>1</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="5">
+        <v>4</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G35" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H35" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="K35" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="L35" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G35" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H35" s="7">
+      <c r="M35" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N35" s="6">
         <v>1712823</v>
       </c>
-      <c r="I35" s="6" t="s">
+      <c r="O35" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="J35" s="6" t="s">
+      <c r="P35" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="K35" s="6"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="8">
-        <v>1</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C36" s="8" t="s">
+      <c r="Q35" s="5"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>1</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="7">
+        <v>2</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G36" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H36" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I36" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J36" s="8">
         <v>100</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="K36" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="L36" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="M36" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="H36" s="9" t="s">
+      <c r="N36" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="I36" s="8" t="s">
+      <c r="O36" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="J36" s="8" t="s">
+      <c r="P36" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="K36" s="8"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
+      <c r="Q36" s="7"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
         <v>4</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C37" s="6" t="s">
+      <c r="B37" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="5">
+        <v>2</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G37" s="5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H37" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I37" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="K37" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="L37" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="M37" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="H37" s="7" t="s">
+      <c r="N37" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="I37" s="6" t="s">
+      <c r="O37" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="J37" s="6" t="s">
+      <c r="P37" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="K37" s="6"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
+      <c r="Q37" s="5"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
         <v>4</v>
       </c>
-      <c r="B38" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C38" s="8" t="s">
+      <c r="B38" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D38" s="7">
+        <v>2</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G38" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H38" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I38" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="K38" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="L38" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="G38" s="8" t="s">
+      <c r="M38" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="H38" s="9" t="s">
+      <c r="N38" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="I38" s="8" t="s">
+      <c r="O38" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="J38" s="8" t="s">
+      <c r="P38" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="K38" s="8" t="s">
+      <c r="Q38" s="7" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="6">
-        <v>2</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C39" s="6" t="s">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>2</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="5">
+        <v>2</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G39" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H39" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="K39" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="L39" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="G39" s="6" t="s">
+      <c r="M39" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="H39" s="7" t="s">
+      <c r="N39" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="I39" s="6" t="s">
+      <c r="O39" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="J39" s="6" t="s">
+      <c r="P39" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="K39" s="6"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="8">
+      <c r="Q39" s="5"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
         <v>3</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C40" s="8" t="s">
+      <c r="B40" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D40" s="7">
+        <v>2</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G40" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H40" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I40" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J40" s="8">
         <v>200</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="K40" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="L40" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="G40" s="8" t="s">
+      <c r="M40" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="H40" s="9" t="s">
+      <c r="N40" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="I40" s="8" t="s">
+      <c r="O40" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="J40" s="8" t="s">
+      <c r="P40" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="K40" s="8"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="6">
+      <c r="Q40" s="7"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
         <v>5</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C41" s="6" t="s">
+      <c r="B41" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="5">
+        <v>2</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G41" s="5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H41" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I41" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J41" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="K41" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="L41" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="M41" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="H41" s="7" t="s">
+      <c r="N41" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="I41" s="6" t="s">
+      <c r="O41" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="J41" s="6" t="s">
+      <c r="P41" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="K41" s="6"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="8">
-        <v>1</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C42" s="8" t="s">
+      <c r="Q41" s="5"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
+        <v>1</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D42" s="7">
+        <v>2</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G42" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H42" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I42" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J42" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="K42" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="L42" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="G42" s="8" t="s">
+      <c r="M42" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="H42" s="9" t="s">
+      <c r="N42" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="I42" s="8" t="s">
+      <c r="O42" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="J42" s="8" t="s">
+      <c r="P42" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="K42" s="8"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="6">
-        <v>2</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C43" s="6" t="s">
+      <c r="Q42" s="7"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>2</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D43" s="5">
+        <v>2</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G43" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H43" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I43" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J43" s="6">
         <v>10</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="K43" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="L43" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="M43" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="H43" s="7" t="s">
+      <c r="N43" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="I43" s="6" t="s">
+      <c r="O43" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="J43" s="6" t="s">
+      <c r="P43" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="K43" s="6"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="8">
+      <c r="Q43" s="5"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
         <v>4</v>
       </c>
-      <c r="B44" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C44" s="8" t="s">
+      <c r="B44" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D44" s="7">
+        <v>2</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G44" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H44" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I44" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J44" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="K44" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="L44" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="G44" s="8" t="s">
+      <c r="M44" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="H44" s="9" t="s">
+      <c r="N44" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="I44" s="8" t="s">
+      <c r="O44" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="J44" s="8" t="s">
+      <c r="P44" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="K44" s="8"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="6">
-        <v>1</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C45" s="6" t="s">
+      <c r="Q44" s="7"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>1</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="5">
+        <v>2</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G45" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H45" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I45" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J45" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="K45" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="L45" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="G45" s="6" t="s">
+      <c r="M45" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="H45" s="7" t="s">
+      <c r="N45" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="I45" s="6" t="s">
+      <c r="O45" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="J45" s="6" t="s">
+      <c r="P45" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="K45" s="6" t="s">
+      <c r="Q45" s="5" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="8">
-        <v>1</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C46" s="8" t="s">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
+        <v>1</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D46" s="7">
+        <v>2</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G46" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H46" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I46" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J46" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="K46" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="L46" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="G46" s="8" t="s">
+      <c r="M46" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="H46" s="9" t="s">
+      <c r="N46" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="I46" s="8" t="s">
+      <c r="O46" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="J46" s="8" t="s">
+      <c r="P46" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="K46" s="8"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="6">
-        <v>2</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C47" s="6" t="s">
+      <c r="Q46" s="7"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>2</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="5">
+        <v>2</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G47" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H47" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I47" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J47" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="K47" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="L47" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="G47" s="6" t="s">
+      <c r="M47" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="H47" s="7" t="s">
+      <c r="N47" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="I47" s="6" t="s">
+      <c r="O47" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="J47" s="6" t="s">
+      <c r="P47" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="K47" s="6" t="s">
+      <c r="Q47" s="5" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="8">
-        <v>2</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C48" s="8" t="s">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
+        <v>2</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D48" s="9">
+      <c r="D48" s="7">
+        <v>2</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G48" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H48" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J48" s="8">
         <v>5</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="K48" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F48" s="8" t="s">
+      <c r="L48" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="G48" s="8" t="s">
+      <c r="M48" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="H48" s="9" t="s">
+      <c r="N48" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="I48" s="8" t="s">
+      <c r="O48" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="J48" s="8" t="s">
+      <c r="P48" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="K48" s="8" t="s">
+      <c r="Q48" s="7" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="6">
-        <v>1</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C49" s="6" t="s">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <v>1</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D49" s="5">
+        <v>2</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G49" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H49" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I49" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J49" s="6">
         <v>0.01</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="K49" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F49" s="6" t="s">
+      <c r="L49" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="G49" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H49" s="7">
+      <c r="M49" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N49" s="6">
         <v>2079429</v>
       </c>
-      <c r="I49" s="6" t="s">
+      <c r="O49" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="J49" s="6" t="s">
+      <c r="P49" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="K49" s="6"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="8">
-        <v>1</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C50" s="8" t="s">
+      <c r="Q49" s="5"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>1</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D50" s="7">
+        <v>2</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G50" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H50" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I50" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J50" s="8">
         <v>0.1</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="K50" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F50" s="8" t="s">
+      <c r="L50" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="G50" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H50" s="9">
+      <c r="M50" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N50" s="8">
         <v>1865265</v>
       </c>
-      <c r="I50" s="8" t="s">
+      <c r="O50" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="J50" s="8" t="s">
+      <c r="P50" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="K50" s="8"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="6">
-        <v>1</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C51" s="6" t="s">
+      <c r="Q50" s="7"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
+        <v>1</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="7"/>
-      <c r="E51" s="6" t="s">
+      <c r="D51" s="5">
+        <v>3</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G51" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H51" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I51" s="5">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="J51" s="6"/>
+      <c r="K51" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="L51" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G51" s="6" t="s">
+      <c r="M51" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="H51" s="7" t="s">
+      <c r="N51" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="I51" s="6" t="s">
+      <c r="O51" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="J51" s="6" t="s">
+      <c r="P51" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="K51" s="6"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="8">
-        <v>1</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C52" s="8" t="s">
+      <c r="Q51" s="5"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <v>1</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D52" s="9"/>
-      <c r="E52" s="8" t="s">
+      <c r="D52" s="7">
+        <v>3</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G52" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H52" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I52" s="7">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="J52" s="8"/>
+      <c r="K52" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="L52" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G52" s="8" t="s">
+      <c r="M52" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H52" s="9" t="s">
+      <c r="N52" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I52" s="8" t="s">
+      <c r="O52" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J52" s="9" t="s">
+      <c r="P52" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K52" s="8"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="6">
-        <v>1</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C53" s="6" t="s">
+      <c r="Q52" s="7"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53" s="5">
+        <v>1</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D53" s="7"/>
-      <c r="E53" s="6" t="s">
+      <c r="D53" s="5">
+        <v>3</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G53" s="5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H53" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I53" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J53" s="6"/>
+      <c r="K53" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F53" s="6" t="s">
+      <c r="L53" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="G53" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H53" s="7">
+      <c r="M53" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N53" s="6">
         <v>1081232</v>
       </c>
-      <c r="I53" s="6" t="s">
+      <c r="O53" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="J53" s="6" t="s">
+      <c r="P53" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="K53" s="6"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="8">
-        <v>1</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C54" s="8" t="s">
+      <c r="Q53" s="5"/>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
+        <v>1</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C54" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D54" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="F54" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="G54" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H54" s="9">
-        <v>1904027</v>
-      </c>
-      <c r="I54" s="8" t="s">
-        <v>188</v>
+      <c r="D54" s="7">
+        <v>3</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G54" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H54" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I54" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J54" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="K54" s="8"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="6">
-        <v>2</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C55" s="6" t="s">
+      <c r="K54" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="L54" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="M54" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N54" s="8">
+        <v>1904027</v>
+      </c>
+      <c r="O54" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="P54" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q54" s="7"/>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" s="5">
+        <v>2</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="5">
+        <v>8</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G55" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H55" s="5">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I55" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J55" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E55" s="6" t="s">
+      <c r="K55" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F55" s="6" t="s">
+      <c r="L55" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G55" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H55" s="7">
+      <c r="M55" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N55" s="6">
         <v>9845275</v>
       </c>
-      <c r="I55" s="6" t="s">
+      <c r="O55" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="J55" s="6" t="s">
+      <c r="P55" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="K55" s="6"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="8">
-        <v>1</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C56" s="8" t="s">
+      <c r="Q55" s="5"/>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
+        <v>1</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C56" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D56" s="9" t="s">
+      <c r="D56" s="7">
+        <v>6</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G56" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H56" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I56" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J56" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="K56" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H56" s="9">
+      <c r="L56" s="7"/>
+      <c r="M56" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N56" s="8">
         <v>1469178</v>
       </c>
-      <c r="I56" s="8" t="s">
+      <c r="O56" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="J56" s="8" t="s">
+      <c r="P56" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="K56" s="8"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="6">
+      <c r="Q56" s="7"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57" s="5">
         <v>4</v>
       </c>
-      <c r="B57" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C57" s="6" t="s">
+      <c r="B57" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="5">
+        <v>3</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G57" s="5">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H57" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I57" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J57" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="K57" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="F57" s="6" t="s">
+      <c r="L57" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="G57" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H57" s="7">
+      <c r="M57" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N57" s="6">
         <v>1713823</v>
       </c>
-      <c r="I57" s="6" t="s">
+      <c r="O57" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="J57" s="6" t="s">
+      <c r="P57" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="K57" s="6"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="8">
-        <v>1</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C58" s="8" t="s">
+      <c r="Q57" s="5"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
+        <v>1</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C58" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D58" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="E58" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F58" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="G58" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H58" s="9">
-        <v>1754261</v>
-      </c>
-      <c r="I58" s="8" t="s">
-        <v>106</v>
+      <c r="D58" s="7">
+        <v>6</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G58" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H58" s="7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I58" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J58" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="K58" s="8"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="6">
-        <v>1</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C59" s="6" t="s">
+      <c r="K58" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="L58" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="M58" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N58" s="8">
+        <v>1754261</v>
+      </c>
+      <c r="O58" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="P58" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q58" s="7"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59" s="5">
+        <v>1</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="5">
+        <v>8</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G59" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H59" s="5">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I59" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J59" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="K59" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F59" s="6"/>
-      <c r="G59" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H59" s="7">
+      <c r="L59" s="5"/>
+      <c r="M59" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N59" s="6">
         <v>1525544</v>
       </c>
-      <c r="I59" s="6" t="s">
+      <c r="O59" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="J59" s="6" t="s">
+      <c r="P59" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="K59" s="6"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="8">
-        <v>1</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C60" s="8" t="s">
+      <c r="Q59" s="5"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
+        <v>1</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C60" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="D60" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="F60" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="G60" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H60" s="9">
-        <v>1296592</v>
-      </c>
-      <c r="I60" s="8" t="s">
-        <v>127</v>
+      <c r="D60" s="7">
+        <v>3</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G60" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H60" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I60" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J60" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="K60" s="8"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="10">
-        <v>2</v>
-      </c>
-      <c r="B61" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="C61" s="10" t="s">
+      <c r="K60" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="L60" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="M60" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N60" s="8">
+        <v>1296592</v>
+      </c>
+      <c r="O60" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="P60" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q60" s="7"/>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61" s="9">
+        <v>2</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="C61" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D61" s="11" t="s">
+      <c r="D61" s="17">
+        <v>6</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="F61" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="G61" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H61" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I61" s="17">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="J61" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E61" s="10" t="s">
+      <c r="K61" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="F61" s="10" t="s">
+      <c r="L61" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="G61" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H61" s="11">
+      <c r="M61" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="N61" s="10">
         <v>2112372</v>
       </c>
-      <c r="I61" s="10" t="s">
+      <c r="O61" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="J61" s="10" t="s">
+      <c r="P61" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="K61" s="10"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+      <c r="Q61" s="9"/>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A64" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="B64" s="4"/>
+      <c r="B64" s="15"/>
       <c r="C64">
         <f>COUNTIF(B7:B61,"Y")</f>
         <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="B65" s="4"/>
+      <c r="B65" s="15"/>
       <c r="C65">
         <f>SUMIF(B7:B61,"Y",A7:A61)</f>
         <v>96</v>
       </c>
     </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="B67" s="15"/>
+      <c r="C67">
+        <f>SUM(G7:G61)</f>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="B68" s="15"/>
+      <c r="C68">
+        <f>SUM(H7:H61)</f>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="B69" s="15"/>
+      <c r="C69">
+        <f>SUM(I7:I61)</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D6:F6"/>
+  <mergeCells count="7">
+    <mergeCell ref="J6:L6"/>
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="A1:P2"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
BOM updated with Prices
</commit_message>
<xml_diff>
--- a/Hardware/production/home_bom.xlsx
+++ b/Hardware/production/home_bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="288">
   <si>
     <t>Qty</t>
   </si>
@@ -605,12 +605,6 @@
     <t>RSS090P03</t>
   </si>
   <si>
-    <t>Rohm</t>
-  </si>
-  <si>
-    <t>RSS090P03FU6TB</t>
-  </si>
-  <si>
     <t>STMicroelectronics</t>
   </si>
   <si>
@@ -849,13 +843,62 @@
   </si>
   <si>
     <t>IC SMT Pads</t>
+  </si>
+  <si>
+    <t>Ordered</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Safety</t>
+  </si>
+  <si>
+    <t>Order Quantity</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Per Unit</t>
+  </si>
+  <si>
+    <t>Purchased from Mouser: 511-STM32F050C6T6A</t>
+  </si>
+  <si>
+    <t>Shipped with Matt Douthwaite order</t>
+  </si>
+  <si>
+    <t>Also requires Switch cap. Farnell: 9561552</t>
+  </si>
+  <si>
+    <t>Used in place of RSS090P03FU6TB (1525544)</t>
+  </si>
+  <si>
+    <t>SI4431CDY-T1-GE3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -876,6 +919,26 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -940,10 +1003,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -973,18 +1038,544 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="23">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -995,6 +1586,46 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A6:U61" totalsRowShown="0" headerRowDxfId="5" dataDxfId="6">
+  <autoFilter ref="A6:U61"/>
+  <tableColumns count="21">
+    <tableColumn id="1" name="Qty" dataDxfId="22"/>
+    <tableColumn id="2" name="Populate" dataDxfId="21"/>
+    <tableColumn id="3" name="Reference Designator" dataDxfId="20"/>
+    <tableColumn id="4" name="Pins" dataDxfId="19"/>
+    <tableColumn id="5" name="SMT?" dataDxfId="18"/>
+    <tableColumn id="6" name="IC?" dataDxfId="17"/>
+    <tableColumn id="7" name="SMT Pads" dataDxfId="16">
+      <calculatedColumnFormula>IF(B7="Y",IF(E7="Y",IF(F7="N",D7*A7,0),0),0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="IC Pads" dataDxfId="15">
+      <calculatedColumnFormula>IF(B7="Y",IF(E7="Y",IF(F7="Y",D7*A7,0),0),0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="TH Pads" dataDxfId="14">
+      <calculatedColumnFormula>IF(B7="Y",IF(E7="N",D7*A7,0),0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" name="Item Description" dataDxfId="13"/>
+    <tableColumn id="11" name="Column1" dataDxfId="12"/>
+    <tableColumn id="12" name="Column2" dataDxfId="11"/>
+    <tableColumn id="13" name="Supplier" dataDxfId="10"/>
+    <tableColumn id="14" name="Supplier Part No" dataDxfId="9"/>
+    <tableColumn id="15" name="Manufacturer" dataDxfId="8"/>
+    <tableColumn id="16" name="Manufacturer Part No" dataDxfId="7"/>
+    <tableColumn id="17" name="Notes" dataDxfId="4"/>
+    <tableColumn id="20" name="Unit Price" dataDxfId="2"/>
+    <tableColumn id="19" name="Order Quantity" dataDxfId="3">
+      <calculatedColumnFormula>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="18" name="Ordered"/>
+    <tableColumn id="21" name="Total Cost" dataDxfId="1" dataCellStyle="Currency">
+      <calculatedColumnFormula>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1260,77 +1891,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q71"/>
+  <dimension ref="A1:U72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="32.85546875" customWidth="1"/>
     <col min="4" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" customWidth="1"/>
-    <col min="7" max="9" width="10" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
     <col min="10" max="10" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="62.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" customWidth="1"/>
-    <col min="14" max="14" width="21.140625" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="21.85546875" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" customWidth="1"/>
+    <col min="16" max="16" width="27.5703125" customWidth="1"/>
     <col min="17" max="17" width="57.7109375" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" style="22" customWidth="1"/>
+    <col min="19" max="19" width="20.5703125" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" customWidth="1"/>
+    <col min="21" max="21" width="15" style="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B4" s="3">
         <v>41472</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
@@ -1341,28 +1978,32 @@
         <v>160</v>
       </c>
       <c r="D6" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="H6" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>269</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>271</v>
       </c>
       <c r="J6" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
+      <c r="K6" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>275</v>
+      </c>
       <c r="M6" s="11" t="s">
         <v>162</v>
       </c>
@@ -1376,10 +2017,22 @@
         <v>169</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+      <c r="R6" s="23" t="s">
+        <v>279</v>
+      </c>
+      <c r="S6" s="20" t="s">
+        <v>278</v>
+      </c>
+      <c r="T6" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="U6" s="28" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>1</v>
       </c>
@@ -1430,8 +2083,22 @@
         <v>190</v>
       </c>
       <c r="Q7" s="12"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" s="24">
+        <v>0.41</v>
+      </c>
+      <c r="S7" s="21">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T7">
+        <v>83</v>
+      </c>
+      <c r="U7" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>34.03</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>1</v>
       </c>
@@ -1481,11 +2148,25 @@
         <v>176</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="Q8" s="7"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8" s="25">
+        <v>1.02</v>
+      </c>
+      <c r="S8" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T8">
+        <v>83</v>
+      </c>
+      <c r="U8" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>84.66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>1</v>
       </c>
@@ -1536,8 +2217,22 @@
         <v>187</v>
       </c>
       <c r="Q9" s="5"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9" s="26">
+        <v>0.27</v>
+      </c>
+      <c r="S9" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T9">
+        <v>83</v>
+      </c>
+      <c r="U9" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>22.41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>2</v>
       </c>
@@ -1575,7 +2270,7 @@
         <v>75</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="M10" s="7" t="s">
         <v>1</v>
@@ -1584,14 +2279,28 @@
         <v>1856141</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="Q10" s="7"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10" s="25">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="S10" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>165</v>
+      </c>
+      <c r="T10">
+        <v>200</v>
+      </c>
+      <c r="U10" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>3.4000000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8</v>
       </c>
@@ -1629,23 +2338,32 @@
         <v>37</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N11" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="P11" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="O11" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>219</v>
-      </c>
       <c r="Q11" s="5"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11" s="26"/>
+      <c r="S11" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>660</v>
+      </c>
+      <c r="U11" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>1</v>
       </c>
@@ -1683,7 +2401,7 @@
         <v>32</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="M12" s="7" t="s">
         <v>1</v>
@@ -1698,8 +2416,22 @@
         <v>177</v>
       </c>
       <c r="Q12" s="7"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="S12" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T12">
+        <v>100</v>
+      </c>
+      <c r="U12" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>5</v>
       </c>
@@ -1737,23 +2469,32 @@
         <v>37</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="O13" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="P13" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="P13" s="5" t="s">
-        <v>220</v>
-      </c>
       <c r="Q13" s="5"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13" s="26"/>
+      <c r="S13" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>413</v>
+      </c>
+      <c r="U13" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>2</v>
       </c>
@@ -1791,7 +2532,7 @@
         <v>40</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="M14" s="7" t="s">
         <v>1</v>
@@ -1806,8 +2547,22 @@
         <v>178</v>
       </c>
       <c r="Q14" s="7"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14" s="25">
+        <v>0.21</v>
+      </c>
+      <c r="S14" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>165</v>
+      </c>
+      <c r="T14">
+        <v>170</v>
+      </c>
+      <c r="U14" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>35.699999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>1</v>
       </c>
@@ -1845,7 +2600,7 @@
         <v>61</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="M15" s="5" t="s">
         <v>1</v>
@@ -1860,8 +2615,22 @@
         <v>179</v>
       </c>
       <c r="Q15" s="5"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15" s="26">
+        <v>0.2</v>
+      </c>
+      <c r="S15" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T15">
+        <v>100</v>
+      </c>
+      <c r="U15" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>3</v>
       </c>
@@ -1899,23 +2668,32 @@
         <v>37</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="M16" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="P16" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="N16" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="O16" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="P16" s="7" t="s">
-        <v>224</v>
-      </c>
       <c r="Q16" s="7"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16" s="25"/>
+      <c r="S16" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>248</v>
+      </c>
+      <c r="U16" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>1</v>
       </c>
@@ -1966,8 +2744,22 @@
         <v>184</v>
       </c>
       <c r="Q17" s="5"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17" s="26">
+        <v>0.21</v>
+      </c>
+      <c r="S17" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T17">
+        <v>83</v>
+      </c>
+      <c r="U17" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>17.43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>2</v>
       </c>
@@ -2020,8 +2812,22 @@
         <v>183</v>
       </c>
       <c r="Q18" s="7"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="25">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="S18" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>165</v>
+      </c>
+      <c r="T18">
+        <v>165</v>
+      </c>
+      <c r="U18" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>47.849999999999994</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>1</v>
       </c>
@@ -2074,8 +2880,22 @@
         <v>143</v>
       </c>
       <c r="Q19" s="5"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19" s="26">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="S19" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T19">
+        <v>83</v>
+      </c>
+      <c r="U19" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>7.6360000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>1</v>
       </c>
@@ -2122,14 +2942,28 @@
         <v>1625280</v>
       </c>
       <c r="O20" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="P20" s="7" t="s">
         <v>154</v>
       </c>
       <c r="Q20" s="7"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R20" s="25">
+        <v>0.09</v>
+      </c>
+      <c r="S20" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T20">
+        <v>85</v>
+      </c>
+      <c r="U20" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>7.6499999999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>1</v>
       </c>
@@ -2180,8 +3014,22 @@
         <v>92</v>
       </c>
       <c r="Q21" s="5"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21" s="26">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="S21" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T21">
+        <v>90</v>
+      </c>
+      <c r="U21" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>1</v>
       </c>
@@ -2232,8 +3080,22 @@
         <v>86</v>
       </c>
       <c r="Q22" s="7"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22" s="25">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="S22" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T22">
+        <v>83</v>
+      </c>
+      <c r="U22" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>13.695</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>3</v>
       </c>
@@ -2283,9 +3145,25 @@
       <c r="P23" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="Q23" s="5"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q23" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="R23" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="S23" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>248</v>
+      </c>
+      <c r="T23">
+        <v>248</v>
+      </c>
+      <c r="U23" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>1</v>
       </c>
@@ -2326,22 +3204,31 @@
         <v>119</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N24" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="P24" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q24" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="O24" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="P24" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="Q24" s="7" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R24" s="25"/>
+      <c r="S24" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="U24" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>1</v>
       </c>
@@ -2386,14 +3273,30 @@
         <v>2115059</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="P25" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="Q25" s="5"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q25" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="R25" s="26">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="S25" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T25">
+        <v>83</v>
+      </c>
+      <c r="U25" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>166.82999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>1</v>
       </c>
@@ -2443,11 +3346,25 @@
         <v>188</v>
       </c>
       <c r="P26" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="Q26" s="7"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R26" s="25">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="S26" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T26">
+        <v>83</v>
+      </c>
+      <c r="U26" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>46.480000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>1</v>
       </c>
@@ -2494,14 +3411,28 @@
         <v>8638756</v>
       </c>
       <c r="O27" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="P27" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="Q27" s="5"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R27" s="26">
+        <v>0.71</v>
+      </c>
+      <c r="S27" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T27">
+        <v>100</v>
+      </c>
+      <c r="U27" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>1</v>
       </c>
@@ -2540,20 +3471,29 @@
         <v>12</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N28" s="8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O28" s="7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="P28" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="Q28" s="7"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R28" s="25"/>
+      <c r="S28" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="U28" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>1</v>
       </c>
@@ -2604,8 +3544,22 @@
         <v>173</v>
       </c>
       <c r="Q29" s="5"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R29" s="26">
+        <v>0.21</v>
+      </c>
+      <c r="S29" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T29">
+        <v>85</v>
+      </c>
+      <c r="U29" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>17.849999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>1</v>
       </c>
@@ -2656,8 +3610,22 @@
         <v>181</v>
       </c>
       <c r="Q30" s="7"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R30" s="25">
+        <v>0.59</v>
+      </c>
+      <c r="S30" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T30">
+        <v>83</v>
+      </c>
+      <c r="U30" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>48.97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>1</v>
       </c>
@@ -2707,11 +3675,25 @@
         <v>180</v>
       </c>
       <c r="P31" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Q31" s="5"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R31" s="26">
+        <v>0.64</v>
+      </c>
+      <c r="S31" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T31">
+        <v>83</v>
+      </c>
+      <c r="U31" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>53.120000000000005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>1</v>
       </c>
@@ -2756,10 +3738,19 @@
       <c r="O32" s="7"/>
       <c r="P32" s="7"/>
       <c r="Q32" s="7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+      <c r="R32" s="25"/>
+      <c r="S32" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="U32" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>1</v>
       </c>
@@ -2809,9 +3800,25 @@
       <c r="P33" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="Q33" s="5"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q33" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="R33" s="26">
+        <v>0.2</v>
+      </c>
+      <c r="S33" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T33">
+        <v>83</v>
+      </c>
+      <c r="U33" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>1</v>
       </c>
@@ -2862,8 +3869,22 @@
         <v>185</v>
       </c>
       <c r="Q34" s="7"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R34" s="25">
+        <v>0.33</v>
+      </c>
+      <c r="S34" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T34">
+        <v>100</v>
+      </c>
+      <c r="U34" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>1</v>
       </c>
@@ -2910,14 +3931,28 @@
         <v>1712823</v>
       </c>
       <c r="O35" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="P35" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="Q35" s="5"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R35" s="26">
+        <v>0.62</v>
+      </c>
+      <c r="S35" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T35">
+        <v>83</v>
+      </c>
+      <c r="U35" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>51.46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>1</v>
       </c>
@@ -2955,23 +3990,32 @@
         <v>25</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M36" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N36" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O36" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="P36" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="P36" s="7" t="s">
-        <v>227</v>
-      </c>
       <c r="Q36" s="7"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R36" s="25"/>
+      <c r="S36" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="U36" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>4</v>
       </c>
@@ -3009,23 +4053,32 @@
         <v>25</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="P37" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="Q37" s="5"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R37" s="26"/>
+      <c r="S37" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>330</v>
+      </c>
+      <c r="U37" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>4</v>
       </c>
@@ -3063,25 +4116,34 @@
         <v>25</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M38" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N38" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="O38" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="P38" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q38" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="O38" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="P38" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="Q38" s="7" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R38" s="25"/>
+      <c r="S38" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>330</v>
+      </c>
+      <c r="U38" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>2</v>
       </c>
@@ -3119,23 +4181,32 @@
         <v>25</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="O39" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="P39" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="Q39" s="5"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R39" s="26"/>
+      <c r="S39" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>165</v>
+      </c>
+      <c r="U39" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>3</v>
       </c>
@@ -3173,23 +4244,32 @@
         <v>25</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M40" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N40" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="O40" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="P40" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="Q40" s="7"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R40" s="25"/>
+      <c r="S40" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>248</v>
+      </c>
+      <c r="U40" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>5</v>
       </c>
@@ -3227,23 +4307,32 @@
         <v>25</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N41" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="O41" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="P41" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="Q41" s="5"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R41" s="26"/>
+      <c r="S41" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>413</v>
+      </c>
+      <c r="U41" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>1</v>
       </c>
@@ -3281,23 +4370,32 @@
         <v>25</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M42" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N42" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="O42" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="P42" s="7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="Q42" s="7"/>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R42" s="25"/>
+      <c r="S42" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="U42" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>2</v>
       </c>
@@ -3335,23 +4433,32 @@
         <v>25</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N43" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="O43" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="P43" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="Q43" s="5"/>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R43" s="26"/>
+      <c r="S43" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>165</v>
+      </c>
+      <c r="U43" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>4</v>
       </c>
@@ -3389,23 +4496,32 @@
         <v>25</v>
       </c>
       <c r="L44" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M44" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N44" s="8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="O44" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="P44" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="Q44" s="7"/>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R44" s="25"/>
+      <c r="S44" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>330</v>
+      </c>
+      <c r="U44" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>1</v>
       </c>
@@ -3443,25 +4559,34 @@
         <v>25</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N45" s="6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="O45" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="P45" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="Q45" s="5" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+      <c r="R45" s="26"/>
+      <c r="S45" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="U45" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>1</v>
       </c>
@@ -3499,23 +4624,32 @@
         <v>25</v>
       </c>
       <c r="L46" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M46" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="O46" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="P46" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="Q46" s="7"/>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R46" s="25"/>
+      <c r="S46" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="U46" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>2</v>
       </c>
@@ -3553,25 +4687,34 @@
         <v>25</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N47" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="P47" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="Q47" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="R47" s="26"/>
+      <c r="S47" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>165</v>
+      </c>
+      <c r="U47" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>2</v>
       </c>
@@ -3609,25 +4752,34 @@
         <v>25</v>
       </c>
       <c r="L48" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M48" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N48" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="O48" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="P48" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q48" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="O48" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="P48" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="Q48" s="7" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R48" s="25"/>
+      <c r="S48" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>165</v>
+      </c>
+      <c r="U48" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>1</v>
       </c>
@@ -3665,7 +4817,7 @@
         <v>21</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M49" s="5" t="s">
         <v>1</v>
@@ -3674,14 +4826,28 @@
         <v>2079429</v>
       </c>
       <c r="O49" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="P49" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Q49" s="5"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R49" s="26">
+        <v>0.22</v>
+      </c>
+      <c r="S49" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T49">
+        <v>85</v>
+      </c>
+      <c r="U49" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>1</v>
       </c>
@@ -3719,7 +4885,7 @@
         <v>21</v>
       </c>
       <c r="L50" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M50" s="7" t="s">
         <v>1</v>
@@ -3731,11 +4897,25 @@
         <v>180</v>
       </c>
       <c r="P50" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="Q50" s="7"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R50" s="25">
+        <v>0.12</v>
+      </c>
+      <c r="S50" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T50">
+        <v>100</v>
+      </c>
+      <c r="U50" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>1</v>
       </c>
@@ -3774,20 +4954,29 @@
         <v>12</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N51" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="O51" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="P51" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="O51" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="P51" s="5" t="s">
-        <v>255</v>
-      </c>
       <c r="Q51" s="5"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R51" s="26"/>
+      <c r="S51" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="U51" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>1</v>
       </c>
@@ -3838,8 +5027,22 @@
         <v>9</v>
       </c>
       <c r="Q52" s="7"/>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R52" s="25">
+        <v>0.13</v>
+      </c>
+      <c r="S52" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T52">
+        <v>83</v>
+      </c>
+      <c r="U52" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>10.790000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>1</v>
       </c>
@@ -3890,8 +5093,22 @@
         <v>171</v>
       </c>
       <c r="Q53" s="5"/>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R53" s="26">
+        <v>1.6E-2</v>
+      </c>
+      <c r="S53" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T53">
+        <v>90</v>
+      </c>
+      <c r="U53" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>1</v>
       </c>
@@ -3944,8 +5161,22 @@
         <v>156</v>
       </c>
       <c r="Q54" s="7"/>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R54" s="25">
+        <v>0.34</v>
+      </c>
+      <c r="S54" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T54">
+        <v>83</v>
+      </c>
+      <c r="U54" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>28.220000000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>2</v>
       </c>
@@ -3992,14 +5223,28 @@
         <v>9845275</v>
       </c>
       <c r="O55" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="P55" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="Q55" s="5"/>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R55" s="26">
+        <v>0.42</v>
+      </c>
+      <c r="S55" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>165</v>
+      </c>
+      <c r="T55">
+        <v>165</v>
+      </c>
+      <c r="U55" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>69.3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>1</v>
       </c>
@@ -4050,8 +5295,22 @@
         <v>191</v>
       </c>
       <c r="Q56" s="7"/>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R56" s="25">
+        <v>1.5</v>
+      </c>
+      <c r="S56" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T56">
+        <v>100</v>
+      </c>
+      <c r="U56" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>4</v>
       </c>
@@ -4104,8 +5363,22 @@
         <v>132</v>
       </c>
       <c r="Q57" s="5"/>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R57" s="26">
+        <v>3.9E-2</v>
+      </c>
+      <c r="S57" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>330</v>
+      </c>
+      <c r="T57">
+        <v>330</v>
+      </c>
+      <c r="U57" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>12.87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>1</v>
       </c>
@@ -4158,8 +5431,22 @@
         <v>102</v>
       </c>
       <c r="Q58" s="7"/>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R58" s="25">
+        <v>0.69</v>
+      </c>
+      <c r="S58" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T58">
+        <v>100</v>
+      </c>
+      <c r="U58" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>1</v>
       </c>
@@ -4201,17 +5488,33 @@
         <v>1</v>
       </c>
       <c r="N59" s="6">
-        <v>1525544</v>
+        <v>1858950</v>
       </c>
       <c r="O59" s="5" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="P59" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q59" s="5"/>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+      <c r="Q59" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="R59" s="26">
+        <v>0.41</v>
+      </c>
+      <c r="S59" s="5">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T59">
+        <v>83</v>
+      </c>
+      <c r="U59" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>34.03</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>1</v>
       </c>
@@ -4264,35 +5567,49 @@
         <v>123</v>
       </c>
       <c r="Q60" s="7"/>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R60" s="25">
+        <v>0.24</v>
+      </c>
+      <c r="S60" s="7">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>83</v>
+      </c>
+      <c r="T60">
+        <v>83</v>
+      </c>
+      <c r="U60" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>19.919999999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
         <v>2</v>
       </c>
-      <c r="B61" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="C61" s="17" t="s">
+      <c r="B61" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C61" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="D61" s="17">
+      <c r="D61" s="15">
         <v>6</v>
       </c>
-      <c r="E61" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="F61" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G61" s="17">
+      <c r="E61" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="G61" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H61" s="17">
+      <c r="H61" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I61" s="17">
+      <c r="I61" s="15">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
@@ -4312,28 +5629,58 @@
         <v>2112372</v>
       </c>
       <c r="O61" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="P61" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="Q61" s="9"/>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A64" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="B64" s="15"/>
+      <c r="R61" s="24">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="S61" s="21">
+        <f>ROUNDUP(Table1[[#This Row],[Qty]]*($C$71*(1+$C$72)),0)</f>
+        <v>165</v>
+      </c>
+      <c r="T61">
+        <v>170</v>
+      </c>
+      <c r="U61" s="29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Ordered]]</f>
+        <v>29.070000000000004</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T63" t="s">
+        <v>281</v>
+      </c>
+      <c r="U63" s="27">
+        <f>SUM(Table1[Total Cost])</f>
+        <v>1344.6310000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="B64" s="16"/>
       <c r="C64">
         <f>COUNTIF(B7:B61,"Y")</f>
         <v>54</v>
       </c>
+      <c r="T64" t="s">
+        <v>282</v>
+      </c>
+      <c r="U64" s="27">
+        <f>$U$63/$C$71</f>
+        <v>17.928413333333335</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="B65" s="15"/>
+      <c r="A65" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B65" s="16"/>
       <c r="C65">
         <f>SUMIF(B7:B61,"Y",A7:A61)</f>
         <v>96</v>
@@ -4344,30 +5691,30 @@
       <c r="B66" s="4"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="B67" s="15"/>
+      <c r="A67" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="B67" s="16"/>
       <c r="C67">
         <f>SUM(G7:G61)</f>
         <v>162</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="15" t="s">
-        <v>274</v>
-      </c>
-      <c r="B68" s="15"/>
+      <c r="A68" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="B68" s="16"/>
       <c r="C68">
         <f>SUM(H7:H61)</f>
         <v>94</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="B69" s="15"/>
+      <c r="A69" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B69" s="16"/>
       <c r="C69">
         <f>SUM(I7:I61)</f>
         <v>68</v>
@@ -4378,12 +5725,27 @@
       <c r="B70" s="2"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
+      <c r="A71" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="B71" s="16"/>
+      <c r="C71">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="B72" s="16"/>
+      <c r="C72" s="19">
+        <v>0.1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="J6:L6"/>
+  <mergeCells count="8">
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="A65:B65"/>
     <mergeCell ref="A1:P2"/>
@@ -4393,5 +5755,8 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>